<commit_message>
update planning documents for sprint 1
Co-authored-by: LeaBuchner <lea.buchner@proton.me>
Signed-off-by: engelharddirk <dirk.engelhard@hotmail.de>
</commit_message>
<xml_diff>
--- a/Deliverables/sprint-01/planning-documents.xlsx
+++ b/Deliverables/sprint-01/planning-documents.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="166">
   <si>
     <t>Project Name</t>
   </si>
@@ -216,18 +216,6 @@
     <t>sebastian.knecht@fau.de</t>
   </si>
   <si>
-    <t>Portakal</t>
-  </si>
-  <si>
-    <t>Melih</t>
-  </si>
-  <si>
-    <t>smelihportakal</t>
-  </si>
-  <si>
-    <t>smelihportakal@gmail.com</t>
-  </si>
-  <si>
     <t>Product Owner</t>
   </si>
   <si>
@@ -273,13 +261,19 @@
     <t>Dirk Engelhard</t>
   </si>
   <si>
+    <t>Build process review</t>
+  </si>
+  <si>
     <t>Mid-term due</t>
   </si>
   <si>
-    <t>Demo day!</t>
-  </si>
-  <si>
-    <t>Retrospective</t>
+    <t>Team Workshop</t>
+  </si>
+  <si>
+    <t>No class but team meeting</t>
+  </si>
+  <si>
+    <t>Demo day!+retrospective</t>
   </si>
   <si>
     <t>Product owners, software developers, and Scurm Master are set and ideally don't change over time; the critical part is the Release Manager role you need to define here</t>
@@ -409,9 +403,6 @@
   </si>
   <si>
     <t>Sara Belz</t>
-  </si>
-  <si>
-    <t>Melih Portakal</t>
   </si>
   <si>
     <t>Carlo Strachwitz</t>
@@ -685,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="127">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -803,8 +794,14 @@
     <xf borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
@@ -1300,7 +1297,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B37" displayName="Table_4" name="Table_4" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B36" displayName="Table_4" name="Table_4" id="4">
   <tableColumns count="2">
     <tableColumn name="Goals" id="1"/>
     <tableColumn name="achieve the project goal" id="2"/>
@@ -1547,405 +1544,405 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="E1" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="F1" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="G1" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="65" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="68"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="65" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="66"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="66"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75">
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="77">
         <f>sum(D8:D13)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="77">
         <f>D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6">
-      <c r="A6" s="66"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7">
-      <c r="A7" s="76" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="A7" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="96"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
     </row>
     <row r="8">
-      <c r="A8" s="66"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="68"/>
-      <c r="G8" s="79" t="s">
-        <v>145</v>
+      <c r="A8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="81" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="80">
+      <c r="A9" s="82">
         <v>1.0</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="75">
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="77">
         <f>sum(D16:D21)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="77">
         <f>$D$5</f>
         <v>0</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="77">
         <f>sum(F16:F21)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9" s="77">
         <f>$D$5</f>
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="66">
+      <c r="A10" s="68">
         <f t="shared" ref="A10:A11" si="1">A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="81">
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="83">
         <f>sum(D22:D27)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="81">
+      <c r="E10" s="83">
         <f t="shared" ref="E10:E12" si="2">E9-D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="81">
+      <c r="F10" s="83">
         <f>sum(F22:F27)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="81">
+      <c r="G10" s="83">
         <f t="shared" ref="G10:G12" si="3">G9-F9</f>
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="80">
+      <c r="A11" s="82">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75">
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77">
         <f>sum(D28:D33)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="77">
         <f>sum(F28:F33)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="75">
+      <c r="G11" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="81">
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="68"/>
-      <c r="G12" s="81">
+      <c r="F12" s="70"/>
+      <c r="G12" s="83">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="80"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
     </row>
     <row r="14">
-      <c r="A14" s="84" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="A14" s="86" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="87"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
     </row>
     <row r="15">
-      <c r="A15" s="80"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
     </row>
     <row r="16">
-      <c r="A16" s="87">
+      <c r="A16" s="89">
         <f>A9</f>
         <v>1</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
     </row>
     <row r="17">
-      <c r="A17" s="80"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
     </row>
     <row r="18">
-      <c r="A18" s="66"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="67"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="69"/>
     </row>
     <row r="19">
-      <c r="A19" s="80"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="74"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="76"/>
     </row>
     <row r="20">
-      <c r="A20" s="91"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="83"/>
+      <c r="A20" s="93"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="85"/>
     </row>
     <row r="21">
-      <c r="A21" s="80"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="74"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="76"/>
     </row>
     <row r="22">
-      <c r="A22" s="87">
+      <c r="A22" s="89">
         <f>A10</f>
         <v>2</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
     </row>
     <row r="23">
-      <c r="A23" s="80"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
     </row>
     <row r="24">
-      <c r="A24" s="91"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="83"/>
+      <c r="A24" s="93"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="85"/>
     </row>
     <row r="25">
-      <c r="A25" s="80"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="74"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="76"/>
     </row>
     <row r="26">
-      <c r="A26" s="91"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="83"/>
+      <c r="A26" s="93"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="85"/>
     </row>
     <row r="27">
-      <c r="A27" s="80"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="74"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="76"/>
     </row>
     <row r="28">
-      <c r="A28" s="87">
+      <c r="A28" s="89">
         <f>A11</f>
         <v>3</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
     </row>
     <row r="29">
-      <c r="A29" s="80"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
     </row>
     <row r="30">
-      <c r="A30" s="91"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
+      <c r="A30" s="93"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
     </row>
     <row r="31">
-      <c r="A31" s="80"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
+      <c r="A31" s="82"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
     </row>
     <row r="32">
-      <c r="A32" s="91"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
+      <c r="A32" s="93"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="85"/>
     </row>
     <row r="33">
-      <c r="A33" s="80"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="92" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="77"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
     </row>
     <row r="34">
-      <c r="A34" s="91"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1973,17 +1970,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="96" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="63" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="97" t="s">
-        <v>150</v>
+      <c r="A1" s="98" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="99" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2">
@@ -2127,10 +2124,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2">
@@ -2240,22 +2237,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2">
@@ -2437,308 +2434,308 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="98" t="str">
+      <c r="A1" s="100" t="str">
         <f>'Project Team'!A1</f>
         <v>Last Name</v>
       </c>
-      <c r="B1" s="98" t="str">
+      <c r="B1" s="100" t="str">
         <f>'Project Team'!B1</f>
         <v>First Name</v>
       </c>
-      <c r="C1" s="99" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
+      <c r="C1" s="101" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="102"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
     </row>
     <row r="2">
-      <c r="A2" s="104" t="str">
+      <c r="A2" s="106" t="str">
         <f>'Project Team'!A2</f>
         <v>Lorenz</v>
       </c>
-      <c r="B2" s="104" t="str">
+      <c r="B2" s="106" t="str">
         <f>'Project Team'!B2</f>
         <v>Alexander</v>
       </c>
-      <c r="C2" s="105">
+      <c r="C2" s="107">
         <v>5.0</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107">
+      <c r="D2" s="108"/>
+      <c r="E2" s="109">
         <f>average(C2:C10)</f>
         <v>5</v>
       </c>
-      <c r="F2" s="108" t="str">
+      <c r="F2" s="110" t="str">
         <f>if(stdev(C2:C7) &gt; 0,"NOK", "OK")</f>
         <v>OK</v>
       </c>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
     </row>
     <row r="3">
-      <c r="A3" s="110" t="str">
+      <c r="A3" s="112" t="str">
         <f>'Project Team'!A3</f>
         <v>Buchner</v>
       </c>
-      <c r="B3" s="110" t="str">
+      <c r="B3" s="112" t="str">
         <f>'Project Team'!B3</f>
         <v>Lea</v>
       </c>
-      <c r="C3" s="105">
+      <c r="C3" s="107">
         <v>5.0</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
+      <c r="D3" s="113"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
     </row>
     <row r="4">
-      <c r="A4" s="104" t="str">
+      <c r="A4" s="106" t="str">
         <f>'Project Team'!A4</f>
         <v>Engelhard</v>
       </c>
-      <c r="B4" s="104" t="str">
+      <c r="B4" s="106" t="str">
         <f>'Project Team'!B4</f>
         <v>Dirk</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="106"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="108"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
     </row>
     <row r="5">
-      <c r="A5" s="110" t="str">
+      <c r="A5" s="112" t="str">
         <f>'Project Team'!A5</f>
         <v>Strachwitz</v>
       </c>
-      <c r="B5" s="110" t="str">
+      <c r="B5" s="112" t="str">
         <f>'Project Team'!B5</f>
         <v>Carlo</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
     </row>
     <row r="6">
-      <c r="A6" s="104" t="str">
+      <c r="A6" s="106" t="str">
         <f>'Project Team'!A6</f>
         <v>Belz</v>
       </c>
-      <c r="B6" s="104" t="str">
+      <c r="B6" s="106" t="str">
         <f>'Project Team'!B6</f>
         <v>Sara</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="117">
+      <c r="C6" s="115"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="119">
         <v>0.0</v>
       </c>
-      <c r="F6" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
+      <c r="F6" s="120" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
     </row>
     <row r="7">
-      <c r="A7" s="110" t="str">
+      <c r="A7" s="112" t="str">
         <f>'Project Team'!A7</f>
         <v>Becker</v>
       </c>
-      <c r="B7" s="110" t="str">
+      <c r="B7" s="112" t="str">
         <f>'Project Team'!B7</f>
         <v>Eugen</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="117">
+      <c r="C7" s="115"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="119">
         <v>1.0</v>
       </c>
-      <c r="F7" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
+      <c r="F7" s="120" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
     </row>
     <row r="8">
-      <c r="A8" s="104" t="str">
+      <c r="A8" s="106" t="str">
         <f>'Project Team'!A8</f>
         <v>Hofmann</v>
       </c>
-      <c r="B8" s="104" t="str">
+      <c r="B8" s="106" t="str">
         <f>'Project Team'!B8</f>
         <v>Leo</v>
       </c>
-      <c r="C8" s="114"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="117">
+      <c r="C8" s="116"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="119">
         <v>2.0</v>
       </c>
-      <c r="F8" s="118" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
+      <c r="F8" s="120" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
     </row>
     <row r="9">
-      <c r="A9" s="110" t="str">
+      <c r="A9" s="112" t="str">
         <f>'Project Team'!A9</f>
         <v>Knecht</v>
       </c>
-      <c r="B9" s="110" t="str">
+      <c r="B9" s="112" t="str">
         <f>'Project Team'!B9</f>
         <v>Sebastian</v>
       </c>
-      <c r="C9" s="114"/>
-      <c r="D9" s="115"/>
-      <c r="E9" s="117">
+      <c r="C9" s="116"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="119">
         <v>3.0</v>
       </c>
-      <c r="F9" s="118" t="s">
+      <c r="F9" s="120" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="106" t="str">
+        <f>'Project Team'!A10</f>
+        <v/>
+      </c>
+      <c r="B10" s="106" t="str">
+        <f>'Project Team'!B10</f>
+        <v/>
+      </c>
+      <c r="C10" s="116"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="119">
+        <v>5.0</v>
+      </c>
+      <c r="F10" s="120" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="112"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="119">
+        <v>8.0</v>
+      </c>
+      <c r="F11" s="120" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="114"/>
+      <c r="H11" s="114"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="106"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="119">
+        <v>13.0</v>
+      </c>
+      <c r="F12" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="104" t="str">
-        <f>'Project Team'!A10</f>
-        <v>Portakal</v>
-      </c>
-      <c r="B10" s="104" t="str">
-        <f>'Project Team'!B10</f>
-        <v>Melih</v>
-      </c>
-      <c r="C10" s="114"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="117">
-        <v>5.0</v>
-      </c>
-      <c r="F10" s="118" t="s">
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="112"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="121" t="s">
         <v>162</v>
       </c>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="110"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="117">
-        <v>8.0</v>
-      </c>
-      <c r="F11" s="118" t="s">
+      <c r="B14" s="122"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="122"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="123"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="124" t="s">
         <v>163</v>
       </c>
-      <c r="G11" s="112"/>
-      <c r="H11" s="112"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="104"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="117">
-        <v>13.0</v>
-      </c>
-      <c r="F12" s="118" t="s">
+      <c r="B16" s="125"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
+      <c r="H16" s="125"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="126" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="115"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="119" t="s">
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="123"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="124" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="121"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="121"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="121"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="121"/>
-      <c r="H15" s="121"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="122" t="s">
-        <v>166</v>
-      </c>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="123"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="124" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="121"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="122" t="s">
-        <v>168</v>
-      </c>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="123"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="125"/>
+      <c r="H18" s="125"/>
     </row>
     <row r="19">
-      <c r="A19" s="121"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="123"/>
+      <c r="H19" s="123"/>
     </row>
     <row r="20">
-      <c r="A20" s="123"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="123"/>
+      <c r="A20" s="125"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
+      <c r="H20" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2895,18 +2892,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>57</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11">
       <c r="A11" s="23"/>
@@ -3006,7 +2995,7 @@
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E1" s="27"/>
       <c r="F1" s="29"/>
@@ -3015,28 +3004,28 @@
     </row>
     <row r="2">
       <c r="A2" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="F2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="G2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="H2" s="30" t="s">
         <v>62</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -3047,19 +3036,19 @@
         <v>45945.0</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H3" s="34"/>
     </row>
@@ -3072,17 +3061,17 @@
         <v>45952</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H4" s="37"/>
     </row>
@@ -3095,17 +3084,17 @@
         <v>45959</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H5" s="34"/>
     </row>
@@ -3118,19 +3107,21 @@
         <v>45966</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="37"/>
+        <v>66</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="32">
@@ -3141,17 +3132,17 @@
         <v>45973</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H7" s="34"/>
     </row>
@@ -3164,17 +3155,17 @@
         <v>45980</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H8" s="37"/>
     </row>
@@ -3187,20 +3178,20 @@
         <v>45987</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10">
@@ -3212,17 +3203,17 @@
         <v>45994</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H10" s="37"/>
     </row>
@@ -3235,17 +3226,17 @@
         <v>46001</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H11" s="34"/>
     </row>
@@ -3258,19 +3249,21 @@
         <v>46008</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="37"/>
+        <v>66</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="32">
@@ -3280,19 +3273,21 @@
         <v>46029.0</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="34"/>
+        <v>66</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="35">
@@ -3303,17 +3298,17 @@
         <v>46036</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H14" s="37"/>
     </row>
@@ -3326,17 +3321,17 @@
         <v>46043</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H15" s="34"/>
     </row>
@@ -3349,20 +3344,17 @@
         <v>46050</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
@@ -3374,63 +3366,63 @@
         <v>46057</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="40"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="42"/>
+      <c r="H18" s="44"/>
     </row>
     <row r="19">
-      <c r="A19" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="42"/>
+      <c r="A19" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="44"/>
     </row>
     <row r="20">
-      <c r="A20" s="45"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="42"/>
+      <c r="H20" s="44"/>
     </row>
     <row r="21">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
-      <c r="H21" s="42"/>
+      <c r="H21" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3458,260 +3450,252 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>78</v>
+      <c r="A1" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14"/>
-      <c r="B2" s="48" t="s">
-        <v>79</v>
+      <c r="B2" s="50" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="14"/>
-      <c r="B3" s="48" t="s">
-        <v>80</v>
+      <c r="B3" s="50" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14"/>
       <c r="B4" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="14"/>
-      <c r="B6" s="48" t="s">
-        <v>84</v>
+      <c r="B6" s="50" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="14"/>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="50" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="14"/>
-      <c r="B9" s="48" t="s">
-        <v>88</v>
+      <c r="B9" s="50" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="17"/>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="51" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8"/>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="51" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8"/>
-      <c r="B14" s="48" t="s">
-        <v>95</v>
+      <c r="B14" s="50" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8"/>
-      <c r="B15" s="48" t="s">
-        <v>96</v>
+      <c r="B15" s="50" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8"/>
-      <c r="B16" s="48" t="s">
-        <v>97</v>
+      <c r="B16" s="50" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="51" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="49" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="14"/>
-      <c r="B19" s="48" t="s">
-        <v>101</v>
+      <c r="B19" s="50" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8"/>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="51" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="49" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="14"/>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="51" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" s="49" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="14"/>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="51" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="49" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="14"/>
-      <c r="B26" s="48" t="s">
-        <v>111</v>
+      <c r="B26" s="50" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="46" t="s">
-        <v>112</v>
+      <c r="A27" s="48" t="s">
+        <v>110</v>
       </c>
       <c r="B27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>119</v>
+      <c r="A35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3738,23 +3722,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="57" t="s">
         <v>121</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3784,11 +3768,11 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>126</v>
+      <c r="A1" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2">
@@ -3893,141 +3877,141 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="57" t="s">
-        <v>127</v>
+      <c r="A1" s="59" t="s">
+        <v>124</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="58">
+      <c r="A2" s="60">
         <v>1.0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="58">
+      <c r="A3" s="60">
         <f t="shared" ref="A3:A16" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="58">
+      <c r="A4" s="60">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="58">
+      <c r="A5" s="60">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="59" t="s">
-        <v>130</v>
+      <c r="B5" s="61" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="58">
+      <c r="A6" s="60">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="58">
+      <c r="A7" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="58">
+      <c r="A8" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="58">
+      <c r="A9" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="58">
+      <c r="A10" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="58">
+      <c r="A11" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="58">
+      <c r="A12" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="58">
+      <c r="A13" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="58">
+      <c r="A14" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="58">
+      <c r="A15" s="60">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="58">
+      <c r="A16" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="58"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="58"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="60"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="60"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="2"/>
     </row>
   </sheetData>
@@ -4056,132 +4040,132 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="57" t="s">
-        <v>127</v>
+      <c r="A1" s="59" t="s">
+        <v>124</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="58">
+      <c r="A2" s="60">
         <v>1.0</v>
       </c>
       <c r="B2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="58">
+      <c r="A3" s="60">
         <f t="shared" ref="A3:A16" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="58">
+      <c r="A4" s="60">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="58">
+      <c r="A5" s="60">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="58">
+      <c r="A6" s="60">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="58">
+      <c r="A7" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="58">
+      <c r="A8" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="58">
+      <c r="A9" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="58">
+      <c r="A10" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="58">
+      <c r="A11" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="58">
+      <c r="A12" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="58">
+      <c r="A13" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="58">
+      <c r="A14" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="58">
+      <c r="A15" s="60">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="58">
+      <c r="A16" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="58"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="58"/>
-      <c r="B18" s="61" t="s">
-        <v>133</v>
+      <c r="A18" s="60"/>
+      <c r="B18" s="63" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="60"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="60"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="2"/>
     </row>
   </sheetData>
@@ -4211,414 +4195,414 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="E1" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="F1" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="G1" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="65" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="65" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="66"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75">
+      <c r="B5" s="75"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="77">
         <f>sum(D8:D13)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="77">
         <f>D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6">
-      <c r="A6" s="66"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7">
-      <c r="A7" s="76" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="A7" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="79"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
     </row>
     <row r="8">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="68"/>
-      <c r="G8" s="79" t="s">
-        <v>145</v>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="81" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="80">
+      <c r="A9" s="82">
         <v>1.0</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="75">
+      <c r="B9" s="74"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="77">
         <f>sum(D16:D21)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="77">
         <f>$D$5</f>
         <v>0</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="77">
         <f>sum(F16:F21)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9" s="77">
         <f>$D$5</f>
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="66">
+      <c r="A10" s="68">
         <f t="shared" ref="A10:A11" si="1">A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="81">
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="83">
         <f>sum(D22:D27)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="81">
+      <c r="E10" s="83">
         <f t="shared" ref="E10:E12" si="2">E9-D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="81">
+      <c r="F10" s="83">
         <f>sum(F22:F27)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="81">
+      <c r="G10" s="83">
         <f t="shared" ref="G10:G12" si="3">G9-F9</f>
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="80">
+      <c r="A11" s="82">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75">
+      <c r="B11" s="74"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77">
         <f>sum(D28:D33)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="77">
         <f>sum(F28:F33)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="75">
+      <c r="G11" s="77">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="81">
+      <c r="B12" s="85"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="68"/>
-      <c r="G12" s="81">
+      <c r="F12" s="70"/>
+      <c r="G12" s="83">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="80"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
     </row>
     <row r="14">
-      <c r="A14" s="84" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="A14" s="86" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="87"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
     </row>
     <row r="15">
-      <c r="A15" s="80"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
     </row>
     <row r="16">
-      <c r="A16" s="87">
+      <c r="A16" s="89">
         <f t="shared" ref="A16:B16" si="4">A9</f>
         <v>1</v>
       </c>
-      <c r="B16" s="88" t="str">
+      <c r="B16" s="90" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
     </row>
     <row r="17">
-      <c r="A17" s="80"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
     </row>
     <row r="18">
-      <c r="A18" s="66"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="67"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="69"/>
     </row>
     <row r="19">
-      <c r="A19" s="80"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="74"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="76"/>
     </row>
     <row r="20">
-      <c r="A20" s="91"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="83"/>
+      <c r="A20" s="93"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="85"/>
     </row>
     <row r="21">
-      <c r="A21" s="80"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="74"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="76"/>
     </row>
     <row r="22">
-      <c r="A22" s="87">
+      <c r="A22" s="89">
         <f t="shared" ref="A22:B22" si="5">A10</f>
         <v>2</v>
       </c>
-      <c r="B22" s="88" t="str">
+      <c r="B22" s="90" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
     </row>
     <row r="23">
-      <c r="A23" s="80"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
     </row>
     <row r="24">
-      <c r="A24" s="91"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="83"/>
+      <c r="A24" s="93"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="85"/>
     </row>
     <row r="25">
-      <c r="A25" s="80"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="74"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="76"/>
     </row>
     <row r="26">
-      <c r="A26" s="91"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="83"/>
+      <c r="A26" s="93"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="85"/>
     </row>
     <row r="27">
-      <c r="A27" s="80"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="74"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="76"/>
     </row>
     <row r="28">
-      <c r="A28" s="87">
+      <c r="A28" s="89">
         <f t="shared" ref="A28:B28" si="6">A11</f>
         <v>3</v>
       </c>
-      <c r="B28" s="88" t="str">
+      <c r="B28" s="90" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
     </row>
     <row r="29">
-      <c r="A29" s="80"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
     </row>
     <row r="30">
-      <c r="A30" s="91"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
+      <c r="A30" s="93"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
     </row>
     <row r="31">
-      <c r="A31" s="80"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
+      <c r="A31" s="82"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
     </row>
     <row r="32">
-      <c r="A32" s="91"/>
-      <c r="B32" s="83"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
+      <c r="A32" s="93"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="85"/>
     </row>
     <row r="33">
-      <c r="A33" s="80"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="92" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="77"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
     </row>
     <row r="34">
-      <c r="A34" s="91"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>